<commit_message>
stage 6 - web client
</commit_message>
<xml_diff>
--- a/files/accounts.xlsx
+++ b/files/accounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,35 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>test_22@gmail.com</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>test_5@gmail.com</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>test_g2@gmail.com</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>test0@mail.ru</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>v.chuchkanov@gmail.com</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>test_g@gmail.com</t>
         </is>
@@ -458,32 +473,41 @@
     <row r="2">
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>123</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>temp</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>fgh4</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>1234567</t>
         </is>
@@ -492,56 +516,77 @@
     <row r="5">
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
         <is>
           <t>fgh3</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
         <is>
           <t>fgh2</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
         <is>
           <t>jhg2</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
         <is>
           <t>ggg</t>
         </is>

</xml_diff>